<commit_message>
Hitter ZIPS 2021 added
</commit_message>
<xml_diff>
--- a/input/input_temperature_and_vegas.xlsx
+++ b/input/input_temperature_and_vegas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="8280" windowHeight="19120"/>
   </bookViews>
   <sheets>
     <sheet name="tempAndVegas" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>Temperature</t>
-  </si>
-  <si>
     <t>HomeOdds</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>San Francisco Giants</t>
+  </si>
+  <si>
+    <t>temperature</t>
   </si>
 </sst>
 </file>
@@ -407,230 +407,143 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>-120</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <v>-120</v>
-      </c>
-      <c r="D3">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>-120</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5">
-        <v>-120</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>100</v>
-      </c>
-      <c r="C6">
-        <v>-120</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7">
-        <v>-120</v>
-      </c>
-      <c r="D7">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>100</v>
-      </c>
-      <c r="C8">
-        <v>-120</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>100</v>
-      </c>
-      <c r="C9">
-        <v>-120</v>
-      </c>
-      <c r="D9">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>100</v>
-      </c>
-      <c r="C10">
-        <v>-120</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>100</v>
-      </c>
-      <c r="C11">
-        <v>-120</v>
-      </c>
-      <c r="D11">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>-120</v>
-      </c>
-      <c r="D12">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>100</v>
-      </c>
-      <c r="C13">
-        <v>-120</v>
-      </c>
-      <c r="D13">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>100</v>
-      </c>
-      <c r="C14">
-        <v>-120</v>
-      </c>
-      <c r="D14">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>100</v>
-      </c>
-      <c r="C15">
-        <v>-120</v>
-      </c>
-      <c r="D15">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>100</v>
-      </c>
-      <c r="C16">
-        <v>-120</v>
-      </c>
-      <c r="D16">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added homer model to test data script
</commit_message>
<xml_diff>
--- a/input/input_temperature_and_vegas.xlsx
+++ b/input/input_temperature_and_vegas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="8280" windowHeight="19120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8000" windowHeight="18720"/>
   </bookViews>
   <sheets>
     <sheet name="tempAndVegas" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -431,7 +431,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -439,7 +439,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -447,7 +447,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -455,7 +455,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -463,7 +463,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>60</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -471,7 +471,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -479,7 +479,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -487,7 +487,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -495,7 +495,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -503,7 +503,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -511,7 +511,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -519,7 +519,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -527,7 +527,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -535,7 +535,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -543,7 +543,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor adjustments to testing script
</commit_message>
<xml_diff>
--- a/input/input_temperature_and_vegas.xlsx
+++ b/input/input_temperature_and_vegas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="9020" windowHeight="18220"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="8000" windowHeight="15200"/>
   </bookViews>
   <sheets>
     <sheet name="tempAndVegas" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>temperature</t>
   </si>
@@ -30,13 +30,22 @@
     <t>OverUnder</t>
   </si>
   <si>
+    <t>Atlanta Braves</t>
+  </si>
+  <si>
     <t>Toronto Blue Jays</t>
   </si>
   <si>
+    <t>St. Louis Cardinals</t>
+  </si>
+  <si>
+    <t>Baltimore Orioles</t>
+  </si>
+  <si>
     <t>Cleveland Indians</t>
   </si>
   <si>
-    <t>Baltimore Orioles</t>
+    <t>Minnesota Twins</t>
   </si>
   <si>
     <t>Texas Rangers</t>
@@ -45,57 +54,26 @@
     <t>Pittsburgh Pirates</t>
   </si>
   <si>
-    <t>Atlanta Braves</t>
+    <t>Los Angeles Dodgers</t>
   </si>
   <si>
     <t>Houston Astros</t>
   </si>
   <si>
-    <t>St. Louis Cardinals</t>
-  </si>
-  <si>
-    <t>Tampa Bay Rays</t>
-  </si>
-  <si>
-    <t>Minnesota Twins</t>
-  </si>
-  <si>
-    <t>Los Angeles Dodgers</t>
-  </si>
-  <si>
     <t>Arizona Diamondbacks</t>
   </si>
   <si>
     <t>Chicago White Sox</t>
-  </si>
-  <si>
-    <t>San Francisco Giants</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,17 +96,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -444,84 +418,39 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>49</v>
-      </c>
-      <c r="C2">
-        <v>-159</v>
-      </c>
-      <c r="D2">
-        <v>8.5</v>
-      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>54</v>
-      </c>
-      <c r="C3">
-        <v>149</v>
-      </c>
-      <c r="D3">
-        <v>8.5</v>
-      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>45</v>
-      </c>
-      <c r="C4">
-        <v>-168</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>70</v>
-      </c>
-      <c r="C5">
-        <v>-147</v>
-      </c>
-      <c r="D5">
-        <v>9.5</v>
-      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>64</v>
-      </c>
-      <c r="C6">
-        <v>-168</v>
-      </c>
-      <c r="D6">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C7">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7">
-        <v>7.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -529,13 +458,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C8">
-        <v>120</v>
+        <v>-172</v>
       </c>
       <c r="D8">
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -543,102 +472,37 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C9">
-        <v>-118</v>
+        <v>-174</v>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>72</v>
-      </c>
-      <c r="C10">
-        <v>103</v>
-      </c>
-      <c r="D10">
-        <v>7.5</v>
-      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>61</v>
-      </c>
-      <c r="C11">
-        <v>-119</v>
-      </c>
-      <c r="D11">
-        <v>7.5</v>
-      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>72</v>
-      </c>
-      <c r="C12">
-        <v>210</v>
-      </c>
-      <c r="D12">
-        <v>11.5</v>
-      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
-        <v>61</v>
-      </c>
-      <c r="C13">
-        <v>-199</v>
-      </c>
-      <c r="D13">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>68</v>
-      </c>
-      <c r="C14">
-        <v>111</v>
-      </c>
-      <c r="D14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>54</v>
-      </c>
-      <c r="C15">
-        <v>106</v>
-      </c>
-      <c r="D15">
-        <v>8.5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>